<commit_message>
weitere urls zu zeitungen gefunde, halb durch nrw
</commit_message>
<xml_diff>
--- a/data/Cities.xlsx
+++ b/data/Cities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Pojektarbeit\DataKraken\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B503105-984F-476D-850A-EC1DFA1B6392}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54E1B3A-80D5-4390-BB81-0B76871BCA24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3612" yWindow="17172" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="191">
   <si>
     <t>Name</t>
   </si>
@@ -492,9 +492,6 @@
     <t>Pressemitteilungen von der Stadt</t>
   </si>
   <si>
-    <t xml:space="preserve">Wiesbaden </t>
-  </si>
-  <si>
     <t>FAZ</t>
   </si>
   <si>
@@ -508,13 +505,106 @@
   </si>
   <si>
     <t>zweite quelle offizielle seite der stadt kassel</t>
+  </si>
+  <si>
+    <t>https://www.svz.de/lokales/zeitung-fuer-die-landeshauptstadt/</t>
+  </si>
+  <si>
+    <t>SVZ</t>
+  </si>
+  <si>
+    <t>alle lokalen nachrichten für schwerin</t>
+  </si>
+  <si>
+    <t>https://rathaus.rostock.de/de/informationen_zum_coronavirus_sars_cov_2_und_zu_covid_19/295614</t>
+  </si>
+  <si>
+    <t>Stadt Rostock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stadt Wiesbaden </t>
+  </si>
+  <si>
+    <t>https://www.nordkurier.de/meine-region/neubrandenburg/</t>
+  </si>
+  <si>
+    <t>Alle lokalen nachrichten aus Neubrandenburg</t>
+  </si>
+  <si>
+    <t>Nordkurier</t>
+  </si>
+  <si>
+    <t>https://www.haz.de/nachrichten/coronavirus-in-hannover</t>
+  </si>
+  <si>
+    <t>Hannoversche Allgemeine</t>
+  </si>
+  <si>
+    <t>https://www.braunschweiger-zeitung.de/braunschweig/article228698343/Corona-Braunschweig-inzidenzwert-aktuell-indizenz-coronavirus-infizierte-ausgangssperre-modellstadt-fakten-infos-informationen.html</t>
+  </si>
+  <si>
+    <t>aktuelle zahlen + nachrichten</t>
+  </si>
+  <si>
+    <t>Braunschweiger Zeitung</t>
+  </si>
+  <si>
+    <t>https://www.nwzonline.de/region/corona-im-nordwesten-alle-informationen-zu-covid-19-impfterminen-und-aktuellen-ereignissen-im-nwz-liveblog_a_50,12,248377618.html</t>
+  </si>
+  <si>
+    <t>Nordwest Zeitung</t>
+  </si>
+  <si>
+    <t>https://www.noz.de/lokales/grafschaft-bentheim</t>
+  </si>
+  <si>
+    <t>regional grafschaft bentheim, nordhorn zu klein</t>
+  </si>
+  <si>
+    <t>Neue Osnabrücker Zeitung</t>
+  </si>
+  <si>
+    <t>https://www.nrz.de/staedte/essen/ , https://www.radioessen.de/information/essen.html</t>
+  </si>
+  <si>
+    <t>alle lokalnachrichten essen, coronaticker bei anderer seite hinter paywall</t>
+  </si>
+  <si>
+    <t>Neue Rhein/Ruhr Zeitung, radio essen</t>
+  </si>
+  <si>
+    <t>https://rp-online.de/nrw/staedte/duisburg/, https://www.rundschau-duisburg.de/tag/coronavirus/</t>
+  </si>
+  <si>
+    <t>RP-Online, Rundschau Duisburg</t>
+  </si>
+  <si>
+    <t>alle lokalnachrichten, tag coronavirus - auch über duisburg hinaus</t>
+  </si>
+  <si>
+    <t>https://www.bochum.de/Corona/Aktuelle-Pressemeldungen-zum-Corona-Virus</t>
+  </si>
+  <si>
+    <t>Stadt Bochum</t>
+  </si>
+  <si>
+    <t>https://www.wz.de/suche/corona/</t>
+  </si>
+  <si>
+    <t>über suche weiter nach wuppertal filterbar, automatisierbar???</t>
+  </si>
+  <si>
+    <t>Westdeutsche Zeitung</t>
+  </si>
+  <si>
+    <t>selbe wie wuppertal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,6 +614,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -712,10 +810,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -738,8 +837,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1020,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1073,7 +1176,7 @@
       <c r="E2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="20" t="s">
         <v>117</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -1094,7 +1197,7 @@
       <c r="E3" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="20" t="s">
         <v>114</v>
       </c>
       <c r="G3" s="5"/>
@@ -1113,7 +1216,7 @@
       <c r="E4" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="20" t="s">
         <v>115</v>
       </c>
       <c r="G4" s="5"/>
@@ -1134,7 +1237,7 @@
       <c r="E5" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="20" t="s">
         <v>110</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -1155,7 +1258,7 @@
       <c r="E6" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="21" t="s">
         <v>112</v>
       </c>
       <c r="G6" s="12"/>
@@ -1176,7 +1279,7 @@
       <c r="E7" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="20" t="s">
         <v>119</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -1220,7 +1323,7 @@
       <c r="E9" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="20" t="s">
         <v>125</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -1243,7 +1346,7 @@
       <c r="E10" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="20" t="s">
         <v>128</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -1264,7 +1367,7 @@
       <c r="E11" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="20" t="s">
         <v>131</v>
       </c>
       <c r="G11" s="5"/>
@@ -1283,7 +1386,7 @@
       <c r="E12" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="21" t="s">
         <v>133</v>
       </c>
       <c r="G12" s="12"/>
@@ -1302,7 +1405,7 @@
       <c r="E13" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="22" t="s">
         <v>135</v>
       </c>
       <c r="G13" s="17" t="s">
@@ -1323,7 +1426,7 @@
       <c r="E14" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="20" t="s">
         <v>138</v>
       </c>
       <c r="G14" s="19"/>
@@ -1342,7 +1445,7 @@
       <c r="E15" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="20" t="s">
         <v>140</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -1363,7 +1466,7 @@
       <c r="E16" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="20" t="s">
         <v>143</v>
       </c>
       <c r="G16" s="5"/>
@@ -1384,7 +1487,7 @@
       <c r="E17" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="21" t="s">
         <v>145</v>
       </c>
       <c r="G17" s="12" t="s">
@@ -1405,7 +1508,7 @@
       <c r="E18" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="20" t="s">
         <v>148</v>
       </c>
       <c r="G18" s="5" t="s">
@@ -1426,7 +1529,7 @@
       <c r="E19" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F19" s="21" t="s">
         <v>148</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -1447,7 +1550,7 @@
       <c r="E20" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="22" t="s">
         <v>151</v>
       </c>
       <c r="G20" s="15"/>
@@ -1464,9 +1567,9 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="F21" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>153</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -1485,10 +1588,10 @@
       </c>
       <c r="D22" s="5"/>
       <c r="E22" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>156</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="G22" s="5"/>
     </row>
@@ -1504,13 +1607,13 @@
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="G23" s="12" t="s">
         <v>159</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -1524,9 +1627,15 @@
         <v>56</v>
       </c>
       <c r="D24" s="5"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="5"/>
+      <c r="E24" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
@@ -1539,9 +1648,15 @@
         <v>60</v>
       </c>
       <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="5"/>
+      <c r="E25" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
@@ -1554,9 +1669,15 @@
         <v>79</v>
       </c>
       <c r="D26" s="12"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="12"/>
+      <c r="E26" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
@@ -1569,8 +1690,12 @@
         <v>56</v>
       </c>
       <c r="D27" s="5"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="9"/>
+      <c r="E27" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>169</v>
+      </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -1584,9 +1709,15 @@
         <v>80</v>
       </c>
       <c r="D28" s="5"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="5"/>
+      <c r="E28" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
@@ -1599,9 +1730,15 @@
         <v>79</v>
       </c>
       <c r="D29" s="5"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="5"/>
+      <c r="E29" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
@@ -1616,9 +1753,15 @@
       <c r="D30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="12"/>
+      <c r="E30" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
@@ -1631,9 +1774,15 @@
         <v>78</v>
       </c>
       <c r="D31" s="5"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="5"/>
+      <c r="E31" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
@@ -1646,9 +1795,15 @@
         <v>83</v>
       </c>
       <c r="D32" s="5"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="5"/>
+      <c r="E32" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
@@ -1661,9 +1816,15 @@
         <v>85</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="5"/>
+      <c r="E33" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F33" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
@@ -1676,9 +1837,15 @@
         <v>90</v>
       </c>
       <c r="D34" s="5"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="5"/>
+      <c r="E34" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F34" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
@@ -1736,9 +1903,15 @@
         <v>101</v>
       </c>
       <c r="D38" s="5"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="5"/>
+      <c r="E38" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
@@ -1766,9 +1939,15 @@
         <v>103</v>
       </c>
       <c r="D40" s="5"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="5"/>
+      <c r="E40" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
@@ -1828,9 +2007,15 @@
         <v>56</v>
       </c>
       <c r="D44" s="5"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="5"/>
+      <c r="E44" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F44" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
@@ -2145,7 +2330,39 @@
     <sortCondition ref="C31:C46"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F34" r:id="rId1" xr:uid="{DF1E6AB6-999E-45F1-85C0-D63CD763D08C}"/>
+    <hyperlink ref="F44" r:id="rId2" xr:uid="{B435A3F4-9BE0-4839-B8DE-9A541943C1A4}"/>
+    <hyperlink ref="F33" r:id="rId3" xr:uid="{23EDBD85-598C-4D65-82CB-5868037F7468}"/>
+    <hyperlink ref="F30" r:id="rId4" xr:uid="{C77A154D-546C-42D7-B060-13EB1C1314AA}"/>
+    <hyperlink ref="F27" r:id="rId5" xr:uid="{1F52B2E1-6C6D-413C-B79E-F139DB3F4F45}"/>
+    <hyperlink ref="F15" r:id="rId6" xr:uid="{6E348C1E-9937-4585-9901-85FC272F570D}"/>
+    <hyperlink ref="F16" r:id="rId7" xr:uid="{B2C42307-D0C1-42DD-AC99-6815C2EDD9DB}"/>
+    <hyperlink ref="F17" r:id="rId8" xr:uid="{A7BA4364-75AF-4644-B7B4-8F01EC7B3F40}"/>
+    <hyperlink ref="F18" r:id="rId9" xr:uid="{D6825D06-F990-49C4-B1A9-B83CEB8E901E}"/>
+    <hyperlink ref="F19" r:id="rId10" xr:uid="{A01C08B8-02A6-4781-9ECE-E954C1F0C51A}"/>
+    <hyperlink ref="F20" r:id="rId11" xr:uid="{D3A030B6-8CEF-4024-9C8A-9B99BA066C6C}"/>
+    <hyperlink ref="F21" r:id="rId12" xr:uid="{2F93D996-D8C6-4763-8856-85EA09D44405}"/>
+    <hyperlink ref="F22" r:id="rId13" xr:uid="{9142F6B1-ABD2-4088-BAF9-637FBE357C76}"/>
+    <hyperlink ref="F25" r:id="rId14" xr:uid="{681480CC-2ABC-46A7-A319-19810F57755E}"/>
+    <hyperlink ref="F24" r:id="rId15" xr:uid="{C372BF12-EB8C-4375-8E72-CB22EA91AD16}"/>
+    <hyperlink ref="F26" r:id="rId16" xr:uid="{2C1DC474-FF1B-4623-A0FA-20767EA5DB6D}"/>
+    <hyperlink ref="F28" r:id="rId17" xr:uid="{CB661C54-B89F-48F2-96F2-D12954F37147}"/>
+    <hyperlink ref="F14" r:id="rId18" xr:uid="{92DFB413-3C88-4774-868B-C0A5D797199A}"/>
+    <hyperlink ref="F13" r:id="rId19" xr:uid="{2F936987-D9F4-4987-AFE7-9AFEC25DD48B}"/>
+    <hyperlink ref="F12" r:id="rId20" xr:uid="{72932879-D4F4-4F02-A248-2DB0C2AEA14E}"/>
+    <hyperlink ref="F11" r:id="rId21" xr:uid="{0C47C19A-3BC1-4B91-826D-4D76D7041FCB}"/>
+    <hyperlink ref="F10" r:id="rId22" xr:uid="{EEC3BB12-26F0-4AAB-9FEE-32A3CDE94A0C}"/>
+    <hyperlink ref="F9" r:id="rId23" xr:uid="{2C4E1439-43C5-44B8-9E46-1B78064EBD07}"/>
+    <hyperlink ref="F7" r:id="rId24" xr:uid="{F1F08ED6-803F-49D9-958D-F22B5B1DB091}"/>
+    <hyperlink ref="F6" r:id="rId25" xr:uid="{458AEF0F-FBC8-4B0D-9593-5C1DAD7B01A5}"/>
+    <hyperlink ref="F5" r:id="rId26" xr:uid="{B01B2D09-0D02-4412-880F-930A5EDD7B66}"/>
+    <hyperlink ref="F4" r:id="rId27" xr:uid="{3CE9D3C2-0E99-4ED7-A16E-C502B3EF95E5}"/>
+    <hyperlink ref="F3" r:id="rId28" xr:uid="{CDE6BA0E-70DA-4992-A555-F38558AB277F}"/>
+    <hyperlink ref="F2" r:id="rId29" xr:uid="{1D280004-3FC5-4541-AE68-871A279DBF70}"/>
+    <hyperlink ref="F40" r:id="rId30" xr:uid="{744DB9A3-F86A-46B4-A76B-EB4144A2325A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Bis Dresden weitere zeitungen gesucht
</commit_message>
<xml_diff>
--- a/data/Cities.xlsx
+++ b/data/Cities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Pojektarbeit\DataKraken\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54E1B3A-80D5-4390-BB81-0B76871BCA24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC7C369-14F2-446D-B6EB-F520ECF17959}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3612" yWindow="17172" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="233">
   <si>
     <t>Name</t>
   </si>
@@ -582,22 +582,148 @@
     <t>alle lokalnachrichten, tag coronavirus - auch über duisburg hinaus</t>
   </si>
   <si>
-    <t>https://www.bochum.de/Corona/Aktuelle-Pressemeldungen-zum-Corona-Virus</t>
-  </si>
-  <si>
-    <t>Stadt Bochum</t>
-  </si>
-  <si>
     <t>https://www.wz.de/suche/corona/</t>
   </si>
   <si>
-    <t>über suche weiter nach wuppertal filterbar, automatisierbar???</t>
-  </si>
-  <si>
     <t>Westdeutsche Zeitung</t>
   </si>
   <si>
-    <t>selbe wie wuppertal</t>
+    <t>https://www.nw.de/suche?em_pid=&amp;detail=1&amp;searchressort=&amp;such=corona&amp;em_search_category=all&amp;em_search_details%5B%5D=8259 , https://www.radiobielefeld.de/nachrichten/infos-zum-coronavirus.html</t>
+  </si>
+  <si>
+    <t>über suche gefiltert , radio bielefeld inkl aktueller maßnahmen</t>
+  </si>
+  <si>
+    <t>Neue Westhälische, radio bielefeld</t>
+  </si>
+  <si>
+    <t>https://ga.de/suche/corona/</t>
+  </si>
+  <si>
+    <t>General Anzeiger</t>
+  </si>
+  <si>
+    <t>weiter filterbar, aufruf über api mit suchkriterien im body, json als antwort mit allen artikellinks &lt;3</t>
+  </si>
+  <si>
+    <t>https://www.muensterschezeitung.de/Lokales/Staedte/Muenster/4196231-Corona-Newsticker-aus-der-Region-Nur-Coesfeld-und-Hoexter-liegen-in-NRW-bei-Inzidenzen-unter-100er-Marke</t>
+  </si>
+  <si>
+    <t>Münstersche Zeitung</t>
+  </si>
+  <si>
+    <t>newticker corona</t>
+  </si>
+  <si>
+    <t>https://www.bochum.de/Corona/Aktuelle-Pressemeldungen-zum-Corona-Virus , https://www.lokalkompass.de/tag/corona?loc=bochum</t>
+  </si>
+  <si>
+    <t>Stadt Bochum , lokalkompass</t>
+  </si>
+  <si>
+    <t>https://gelsenkirchener-zeitung.de/category/corona/</t>
+  </si>
+  <si>
+    <t>Gelsenkirchener Zeitung</t>
+  </si>
+  <si>
+    <t>https://www.ruhr24.de/dortmund/corona-in-dortmund-sti1519824/</t>
+  </si>
+  <si>
+    <t>Ruhr24</t>
+  </si>
+  <si>
+    <t>https://www.aachener-zeitung.de/suche/corona/</t>
+  </si>
+  <si>
+    <t>weiter filterbar über request</t>
+  </si>
+  <si>
+    <t>Aachener Zeitung</t>
+  </si>
+  <si>
+    <t>https://www.ksta.de/koeln/corona-in-koeln-sieben-tage-inzidenz-erreicht-hoechstwert---distanzunterricht-ab-montag-36349934</t>
+  </si>
+  <si>
+    <t>Kölner Stadtanzeiger</t>
+  </si>
+  <si>
+    <t>newsticker corona</t>
+  </si>
+  <si>
+    <t>https://www.rheda-wiedenbrueck.de/rathaus/aktuelles/pressemitteilungen/corona/</t>
+  </si>
+  <si>
+    <t>Stadt Rheda Wiedenbrück</t>
+  </si>
+  <si>
+    <t>https://www.kompakt.media/coronavirus-magdeburg-aktuell/</t>
+  </si>
+  <si>
+    <t>Kompakt Media</t>
+  </si>
+  <si>
+    <t>https://hallespektrum.de/tag/corona/</t>
+  </si>
+  <si>
+    <t>Halle Spektrum</t>
+  </si>
+  <si>
+    <t>https://www.shz.de/regionales/kiel/</t>
+  </si>
+  <si>
+    <t>alle lokalnachrichten</t>
+  </si>
+  <si>
+    <t>Schleswig Holsteinischer Zeitungsverlag</t>
+  </si>
+  <si>
+    <t>https://www.shz.de/regionales/luebeck/</t>
+  </si>
+  <si>
+    <t>https://www.shz.de/lokales/flensburger-tageblatt/</t>
+  </si>
+  <si>
+    <t>Flensburger Tageblatt</t>
+  </si>
+  <si>
+    <t>https://www.tlz.de/regionen/erfurt/</t>
+  </si>
+  <si>
+    <t>Thürinigsche Landeszeitung</t>
+  </si>
+  <si>
+    <t>https://www.tlz.de/regionen/jena/</t>
+  </si>
+  <si>
+    <t>https://www.tlz.de/regionen/gera/</t>
+  </si>
+  <si>
+    <t>https://www.saarbruecker-zeitung.de/saarland/saarbruecken/corona-live-ticker-saarland-rki-27543-neuinfektionen-265-todesfaelle_aid-49204663</t>
+  </si>
+  <si>
+    <t>Saarbrückener Zeitung</t>
+  </si>
+  <si>
+    <t>https://www.leipzig.de/jugend-familie-und-soziales/gesundheit/neuartiges-coronavirus-2019-n-cov/</t>
+  </si>
+  <si>
+    <t>Stadt Leipzig</t>
+  </si>
+  <si>
+    <t>artikel auf seite unter allem anderen quatsch</t>
+  </si>
+  <si>
+    <t>Sächsische</t>
+  </si>
+  <si>
+    <t>https://www.saechsische.de/search?q=corona+dresden</t>
+  </si>
+  <si>
+    <t>https://www.saechsische.de/search?q=corona+görlitz</t>
+  </si>
+  <si>
+    <t>suchergebnis aber scheint sortiert</t>
   </si>
 </sst>
 </file>
@@ -814,7 +940,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -833,7 +959,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1123,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58:E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1176,7 +1301,7 @@
       <c r="E2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>117</v>
       </c>
       <c r="G2" s="5" t="s">
@@ -1197,7 +1322,7 @@
       <c r="E3" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>114</v>
       </c>
       <c r="G3" s="5"/>
@@ -1216,7 +1341,7 @@
       <c r="E4" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>115</v>
       </c>
       <c r="G4" s="5"/>
@@ -1237,7 +1362,7 @@
       <c r="E5" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>110</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -1258,7 +1383,7 @@
       <c r="E6" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="20" t="s">
         <v>112</v>
       </c>
       <c r="G6" s="12"/>
@@ -1279,7 +1404,7 @@
       <c r="E7" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>119</v>
       </c>
       <c r="G7" s="5" t="s">
@@ -1303,7 +1428,7 @@
       <c r="F8" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="17" t="s">
         <v>124</v>
       </c>
     </row>
@@ -1323,7 +1448,7 @@
       <c r="E9" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="19" t="s">
         <v>125</v>
       </c>
       <c r="G9" s="5" t="s">
@@ -1346,7 +1471,7 @@
       <c r="E10" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="19" t="s">
         <v>128</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -1367,7 +1492,7 @@
       <c r="E11" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>131</v>
       </c>
       <c r="G11" s="5"/>
@@ -1386,7 +1511,7 @@
       <c r="E12" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="20" t="s">
         <v>133</v>
       </c>
       <c r="G12" s="12"/>
@@ -1405,10 +1530,10 @@
       <c r="E13" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="16" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1426,10 +1551,12 @@
       <c r="E14" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="18" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
@@ -1445,7 +1572,7 @@
       <c r="E15" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="19" t="s">
         <v>140</v>
       </c>
       <c r="G15" s="5" t="s">
@@ -1466,7 +1593,7 @@
       <c r="E16" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="19" t="s">
         <v>143</v>
       </c>
       <c r="G16" s="5"/>
@@ -1487,7 +1614,7 @@
       <c r="E17" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="20" t="s">
         <v>145</v>
       </c>
       <c r="G17" s="12" t="s">
@@ -1508,7 +1635,7 @@
       <c r="E18" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="19" t="s">
         <v>148</v>
       </c>
       <c r="G18" s="5" t="s">
@@ -1529,7 +1656,7 @@
       <c r="E19" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="20" t="s">
         <v>148</v>
       </c>
       <c r="G19" s="5" t="s">
@@ -1550,7 +1677,7 @@
       <c r="E20" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="21" t="s">
         <v>151</v>
       </c>
       <c r="G20" s="15"/>
@@ -1569,7 +1696,7 @@
       <c r="E21" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>153</v>
       </c>
       <c r="G21" s="5" t="s">
@@ -1590,7 +1717,7 @@
       <c r="E22" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="19" t="s">
         <v>156</v>
       </c>
       <c r="G22" s="5"/>
@@ -1630,7 +1757,7 @@
       <c r="E24" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="19" t="s">
         <v>160</v>
       </c>
       <c r="G24" s="5" t="s">
@@ -1651,7 +1778,7 @@
       <c r="E25" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>163</v>
       </c>
       <c r="G25" s="5" t="s">
@@ -1672,7 +1799,7 @@
       <c r="E26" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="20" t="s">
         <v>166</v>
       </c>
       <c r="G26" s="12" t="s">
@@ -1693,7 +1820,7 @@
       <c r="E27" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="19" t="s">
         <v>169</v>
       </c>
       <c r="G27" s="5"/>
@@ -1712,10 +1839,10 @@
       <c r="E28" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="G28" s="19" t="s">
+      <c r="G28" s="18" t="s">
         <v>172</v>
       </c>
     </row>
@@ -1733,7 +1860,7 @@
       <c r="E29" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="F29" s="9" t="s">
+      <c r="F29" s="19" t="s">
         <v>174</v>
       </c>
       <c r="G29" s="5" t="s">
@@ -1756,7 +1883,7 @@
       <c r="E30" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="20" t="s">
         <v>176</v>
       </c>
       <c r="G30" s="12" t="s">
@@ -1817,10 +1944,10 @@
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="F33" s="20" t="s">
-        <v>185</v>
+        <v>197</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>196</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>154</v>
@@ -1838,13 +1965,13 @@
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F34" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -1858,9 +1985,15 @@
         <v>91</v>
       </c>
       <c r="D35" s="5"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="5"/>
+      <c r="E35" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
@@ -1873,9 +2006,15 @@
         <v>94</v>
       </c>
       <c r="D36" s="5"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="5"/>
+      <c r="E36" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
@@ -1888,9 +2027,15 @@
         <v>96</v>
       </c>
       <c r="D37" s="5"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="5"/>
+      <c r="E37" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="G37" s="18" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
@@ -1904,13 +2049,13 @@
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G38" s="12" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1924,8 +2069,12 @@
         <v>102</v>
       </c>
       <c r="D39" s="5"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="9"/>
+      <c r="E39" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>198</v>
+      </c>
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -1940,13 +2089,13 @@
       </c>
       <c r="D40" s="5"/>
       <c r="E40" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F40" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -1960,8 +2109,12 @@
         <v>79</v>
       </c>
       <c r="D41" s="5"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="9"/>
+      <c r="E41" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>200</v>
+      </c>
       <c r="G41" s="5"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
@@ -1977,8 +2130,12 @@
       <c r="D42" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E42" s="4"/>
-      <c r="F42" s="9"/>
+      <c r="E42" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>202</v>
+      </c>
       <c r="G42" s="5"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -1992,9 +2149,15 @@
         <v>60</v>
       </c>
       <c r="D43" s="5"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="5"/>
+      <c r="E43" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="G43" s="18" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
@@ -2008,13 +2171,13 @@
       </c>
       <c r="D44" s="5"/>
       <c r="E44" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="F44" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>185</v>
+      </c>
+      <c r="G44" s="12" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
@@ -2028,9 +2191,15 @@
         <v>87</v>
       </c>
       <c r="D45" s="5"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="5"/>
+      <c r="E45" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
@@ -2043,9 +2212,15 @@
         <v>87</v>
       </c>
       <c r="D46" s="12"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="12"/>
+      <c r="E46" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="F46" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
@@ -2058,8 +2233,12 @@
         <v>56</v>
       </c>
       <c r="D47" s="5"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="9"/>
+      <c r="E47" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>210</v>
+      </c>
       <c r="G47" s="5"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
@@ -2073,8 +2252,12 @@
         <v>60</v>
       </c>
       <c r="D48" s="5"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="9"/>
+      <c r="E48" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>212</v>
+      </c>
       <c r="G48" s="5"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -2103,9 +2286,15 @@
         <v>56</v>
       </c>
       <c r="D50" s="5"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="5"/>
+      <c r="E50" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
@@ -2118,9 +2307,15 @@
         <v>80</v>
       </c>
       <c r="D51" s="5"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="5"/>
+      <c r="E51" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="11" t="s">
@@ -2135,9 +2330,15 @@
       <c r="D52" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="12"/>
+      <c r="E52" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="F52" s="20" t="s">
+        <v>218</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
@@ -2150,9 +2351,15 @@
         <v>56</v>
       </c>
       <c r="D53" s="5"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="5"/>
+      <c r="E53" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
@@ -2165,9 +2372,15 @@
         <v>80</v>
       </c>
       <c r="D54" s="5"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="5"/>
+      <c r="E54" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
@@ -2180,9 +2393,15 @@
         <v>79</v>
       </c>
       <c r="D55" s="12"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="12"/>
+      <c r="E55" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="14" t="s">
@@ -2197,9 +2416,15 @@
       <c r="D56" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="E56" s="14"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="15"/>
+      <c r="E56" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="F56" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="G56" s="16" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
@@ -2212,9 +2437,15 @@
         <v>60</v>
       </c>
       <c r="D57" s="5"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="5"/>
+      <c r="E57" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
@@ -2229,9 +2460,15 @@
       <c r="D58" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E58" s="4"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="5"/>
+      <c r="E58" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
@@ -2244,9 +2481,15 @@
         <v>56</v>
       </c>
       <c r="D59" s="5"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="5"/>
+      <c r="E59" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="11" t="s">
@@ -2333,7 +2576,7 @@
   <hyperlinks>
     <hyperlink ref="F34" r:id="rId1" xr:uid="{DF1E6AB6-999E-45F1-85C0-D63CD763D08C}"/>
     <hyperlink ref="F44" r:id="rId2" xr:uid="{B435A3F4-9BE0-4839-B8DE-9A541943C1A4}"/>
-    <hyperlink ref="F33" r:id="rId3" xr:uid="{23EDBD85-598C-4D65-82CB-5868037F7468}"/>
+    <hyperlink ref="F33" r:id="rId3" display="https://www.bochum.de/Corona/Aktuelle-Pressemeldungen-zum-Corona-Virus" xr:uid="{23EDBD85-598C-4D65-82CB-5868037F7468}"/>
     <hyperlink ref="F30" r:id="rId4" xr:uid="{C77A154D-546C-42D7-B060-13EB1C1314AA}"/>
     <hyperlink ref="F27" r:id="rId5" xr:uid="{1F52B2E1-6C6D-413C-B79E-F139DB3F4F45}"/>
     <hyperlink ref="F15" r:id="rId6" xr:uid="{6E348C1E-9937-4585-9901-85FC272F570D}"/>
@@ -2361,8 +2604,28 @@
     <hyperlink ref="F3" r:id="rId28" xr:uid="{CDE6BA0E-70DA-4992-A555-F38558AB277F}"/>
     <hyperlink ref="F2" r:id="rId29" xr:uid="{1D280004-3FC5-4541-AE68-871A279DBF70}"/>
     <hyperlink ref="F40" r:id="rId30" xr:uid="{744DB9A3-F86A-46B4-A76B-EB4144A2325A}"/>
+    <hyperlink ref="F36" r:id="rId31" xr:uid="{9060DFD2-249E-48FE-91E6-BB3047F47B7E}"/>
+    <hyperlink ref="F41" r:id="rId32" xr:uid="{93C96AA9-76A6-40E9-8152-477EAD204B4A}"/>
+    <hyperlink ref="F39" r:id="rId33" xr:uid="{E899B13B-23E6-4CB0-B0FD-139222896F18}"/>
+    <hyperlink ref="F38" r:id="rId34" xr:uid="{9BC0319B-45C1-4BC5-BD97-F30CBD51D19E}"/>
+    <hyperlink ref="F37" r:id="rId35" xr:uid="{1FFEDBDD-8580-40D5-8704-24A6C0514072}"/>
+    <hyperlink ref="F29" r:id="rId36" xr:uid="{08AF06DC-B205-4858-B335-7EF56BFA78A7}"/>
+    <hyperlink ref="F47" r:id="rId37" xr:uid="{B1B22FED-8945-4B91-B77E-C691E717A38B}"/>
+    <hyperlink ref="F46" r:id="rId38" xr:uid="{A74FFB9C-DCAD-46EC-B74A-0044BD695E45}"/>
+    <hyperlink ref="F45" r:id="rId39" xr:uid="{CFCFB319-8FEA-4F9C-99F0-BDF472037AC2}"/>
+    <hyperlink ref="F42" r:id="rId40" xr:uid="{A97601D5-921E-4E0F-BE35-8FFBAB9C503A}"/>
+    <hyperlink ref="F43" r:id="rId41" xr:uid="{EF1004F3-446F-41F5-9777-45F616ED86BE}"/>
+    <hyperlink ref="F48" r:id="rId42" xr:uid="{50B1C6BB-7ED7-449D-80FA-2BA844C56FEA}"/>
+    <hyperlink ref="F54" r:id="rId43" xr:uid="{5E534BAE-3729-4295-92C6-25D901B9A342}"/>
+    <hyperlink ref="F55" r:id="rId44" xr:uid="{08336736-757F-4BB1-8479-E46E44C39379}"/>
+    <hyperlink ref="F53" r:id="rId45" xr:uid="{1EFBB992-4306-493D-80E6-C857D41D1FEB}"/>
+    <hyperlink ref="F52" r:id="rId46" xr:uid="{5BFA62EF-6C10-405E-860B-3F44626392C0}"/>
+    <hyperlink ref="F51" r:id="rId47" xr:uid="{10107D83-1CDC-4D18-B3F0-E701792A7CF7}"/>
+    <hyperlink ref="F50" r:id="rId48" xr:uid="{9BCC007F-366B-4373-B3BF-1215561D6755}"/>
+    <hyperlink ref="F56" r:id="rId49" xr:uid="{A0C2A79E-654A-4A6D-AC3B-0294B8668277}"/>
+    <hyperlink ref="F58" r:id="rId50" xr:uid="{326AE1F9-6BE8-4CF1-B23E-03EFBB15FF2D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId51"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
started working on basic restriction scraper
</commit_message>
<xml_diff>
--- a/data/Cities.xlsx
+++ b/data/Cities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Pojektarbeit\DataKraken\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jojo\DataKraken\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08099221-D1EA-4982-8BDB-25ADBEB168DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194B489C-289D-4367-A533-7635C05B121C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25560" yWindow="7725" windowWidth="22275" windowHeight="12705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="273">
   <si>
     <t>Name</t>
   </si>
@@ -760,6 +760,90 @@
   </si>
   <si>
     <t>127.0.0.1</t>
+  </si>
+  <si>
+    <t>Maßnahmenquelle</t>
+  </si>
+  <si>
+    <t>https://www.wuerzburg.de/coronainfo/startseite/corona-regelungen/allgemeine-regelungen/index.html</t>
+  </si>
+  <si>
+    <t>wuerzburg.de</t>
+  </si>
+  <si>
+    <t>https://www.muenchen.de/rathaus/Stadtverwaltung/Referat-fuer-Gesundheit-und-Umwelt/Infektionsschutz/Neuartiges_Coronavirus.html#AB</t>
+  </si>
+  <si>
+    <t>muenchen.de</t>
+  </si>
+  <si>
+    <t>hof.de</t>
+  </si>
+  <si>
+    <t>https://www.hof.de/hof/hof_deu/aktuelles/corona-pandemie-02.php</t>
+  </si>
+  <si>
+    <t>FÜR BAYERN</t>
+  </si>
+  <si>
+    <t>https://www.corona-katastrophenschutz.bayern.de/hotspotregionen/index.php</t>
+  </si>
+  <si>
+    <t>https://www.baden-wuerttemberg.de/de/service/aktuelle-infos-zu-corona/aktuelle-corona-verordnung-des-landes-baden-wuerttemberg/</t>
+  </si>
+  <si>
+    <t>Für  BW</t>
+  </si>
+  <si>
+    <t>https://www.swr.de/swraktuell/baden-wuerttemberg/harter-lockdown-folgen-fuer-bw-100.html</t>
+  </si>
+  <si>
+    <t>https://www.berlin.de/corona/massnahmen/</t>
+  </si>
+  <si>
+    <t>https://kkm.brandenburg.de/kkm/de/</t>
+  </si>
+  <si>
+    <t>https://www.bremen.de/corona#inzidenz-aktuell</t>
+  </si>
+  <si>
+    <t>https://www.hamburg.de/verordnung/</t>
+  </si>
+  <si>
+    <t>https://www.hessen.de/fuer-buerger/corona-in-hessen/aktuelle-corona-bestimmungen</t>
+  </si>
+  <si>
+    <t>https://www.ndr.de/nachrichten/mecklenburg-vorpommern/Fragen-und-Antworten-Die-aktuellen-Corona-Regeln-in-MV,coronavirus3470.html</t>
+  </si>
+  <si>
+    <t>https://www.niedersachsen.de/Coronavirus/vorschriften-der-landesregierung-185856.html</t>
+  </si>
+  <si>
+    <t>https://www.land.nrw/de/media/galerie/corona-fakten-1</t>
+  </si>
+  <si>
+    <t>https://coronavirus.sachsen-anhalt.de/</t>
+  </si>
+  <si>
+    <t>https://www.schleswig-holstein.de/DE/Schwerpunkte/Coronavirus/_documents/teaser_erlasse.html</t>
+  </si>
+  <si>
+    <t>https://www.tmasgff.de/covid-19</t>
+  </si>
+  <si>
+    <t>https://www.saarland.de/SharedDocs/Downloads/DE/msgff/download_kontaktbeschraenkung.html</t>
+  </si>
+  <si>
+    <t>https://www.saarland.de/DE/portale/corona/service/rechtsverordnung-massnahmen/rechtsverordnung-massnahmen_node.html</t>
+  </si>
+  <si>
+    <t>https://www.coronavirus.sachsen.de/wir-gegen-corona-8251.html</t>
+  </si>
+  <si>
+    <t>https://corona.rlp.de/de/aktuelles/corona-regeln-im-ueberblick/</t>
+  </si>
+  <si>
+    <t>https://www.radiogong.com/aktuelles/coronazahlen-in-der-region</t>
   </si>
 </sst>
 </file>
@@ -809,7 +893,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1063,12 +1147,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1107,6 +1213,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1388,10 +1496,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <pane xSplit="5" ySplit="30" topLeftCell="G46" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,11 +1511,14 @@
     <col min="2" max="2" width="33.44140625" customWidth="1"/>
     <col min="3" max="4" width="22.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.77734375" customWidth="1"/>
-    <col min="6" max="6" width="107.109375" customWidth="1"/>
-    <col min="7" max="7" width="50.77734375" customWidth="1"/>
+    <col min="6" max="6" width="110.33203125" customWidth="1"/>
+    <col min="7" max="7" width="103.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.21875" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" style="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1426,8 +1540,17 @@
       <c r="G1" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="15" t="s">
         <v>71</v>
       </c>
@@ -1450,7 +1573,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1468,8 +1591,14 @@
         <v>114</v>
       </c>
       <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="I3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1487,8 +1616,11 @@
         <v>115</v>
       </c>
       <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>58</v>
       </c>
@@ -1511,7 +1643,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
@@ -1530,7 +1662,7 @@
       </c>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A7" s="24" t="s">
         <v>75</v>
       </c>
@@ -1552,8 +1684,14 @@
       <c r="G7" s="27" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="I7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>57</v>
       </c>
@@ -1573,8 +1711,14 @@
       <c r="G8" s="10" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="I8" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>69</v>
       </c>
@@ -1597,7 +1741,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>88</v>
       </c>
@@ -1619,8 +1763,14 @@
       <c r="G10" s="4" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="35" t="s">
+        <v>252</v>
+      </c>
+      <c r="I10" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -1638,8 +1788,11 @@
         <v>131</v>
       </c>
       <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>243</v>
       </c>
@@ -1653,8 +1806,14 @@
       <c r="E12" s="3"/>
       <c r="F12" s="9"/>
       <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H12" t="s">
+        <v>247</v>
+      </c>
+      <c r="I12" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="20" t="s">
         <v>6</v>
       </c>
@@ -1673,7 +1832,7 @@
       </c>
       <c r="G13" s="23"/>
     </row>
-    <row r="14" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>7</v>
       </c>
@@ -1693,8 +1852,11 @@
       <c r="G14" s="31" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="I14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>8</v>
       </c>
@@ -1715,7 +1877,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1735,8 +1897,11 @@
       <c r="G16" s="4" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1755,7 +1920,7 @@
       </c>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>11</v>
       </c>
@@ -1778,7 +1943,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>12</v>
       </c>
@@ -1798,8 +1963,11 @@
       <c r="G19" s="27" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>13</v>
       </c>
@@ -1820,7 +1988,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="28" t="s">
         <v>14</v>
       </c>
@@ -1838,8 +2006,11 @@
         <v>150</v>
       </c>
       <c r="G21" s="33"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>15</v>
       </c>
@@ -1860,7 +2031,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
@@ -1878,8 +2049,11 @@
         <v>155</v>
       </c>
       <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
         <v>17</v>
       </c>
@@ -1900,7 +2074,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>18</v>
       </c>
@@ -1921,7 +2095,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>19</v>
       </c>
@@ -1941,8 +2115,11 @@
       <c r="G26" s="11" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I26" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
         <v>20</v>
       </c>
@@ -1963,7 +2140,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>21</v>
       </c>
@@ -1981,8 +2158,11 @@
         <v>168</v>
       </c>
       <c r="G28" s="32"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I28" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>22</v>
       </c>
@@ -2003,7 +2183,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>23</v>
       </c>
@@ -2024,7 +2204,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
         <v>74</v>
       </c>
@@ -2047,7 +2227,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>81</v>
       </c>
@@ -2068,7 +2248,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>82</v>
       </c>
@@ -2088,8 +2268,11 @@
       <c r="G33" s="11" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>84</v>
       </c>
@@ -2110,7 +2293,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>92</v>
       </c>
@@ -2131,7 +2314,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>93</v>
       </c>
@@ -2152,7 +2335,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
@@ -2173,7 +2356,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>97</v>
       </c>
@@ -2194,7 +2377,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>98</v>
       </c>
@@ -2215,7 +2398,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>99</v>
       </c>
@@ -2234,7 +2417,7 @@
       </c>
       <c r="G40" s="11"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>100</v>
       </c>
@@ -2255,7 +2438,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>26</v>
       </c>
@@ -2274,7 +2457,7 @@
       </c>
       <c r="G42" s="11"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>61</v>
       </c>
@@ -2295,7 +2478,7 @@
       </c>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>25</v>
       </c>
@@ -2316,7 +2499,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>24</v>
       </c>
@@ -2337,7 +2520,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>89</v>
       </c>
@@ -2358,7 +2541,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="20" t="s">
         <v>86</v>
       </c>
@@ -2379,7 +2562,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>27</v>
       </c>
@@ -2398,7 +2581,7 @@
       </c>
       <c r="G48" s="32"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>28</v>
       </c>
@@ -2416,8 +2599,11 @@
         <v>211</v>
       </c>
       <c r="G49" s="11"/>
-    </row>
-    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I49" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="20" t="s">
         <v>29</v>
       </c>
@@ -2432,7 +2618,7 @@
       <c r="F50" s="21"/>
       <c r="G50" s="34"/>
     </row>
-    <row r="51" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A51" s="24" t="s">
         <v>30</v>
       </c>
@@ -2453,7 +2639,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>31</v>
       </c>
@@ -2473,8 +2659,11 @@
       <c r="G52" s="11" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I52" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="20" t="s">
         <v>32</v>
       </c>
@@ -2497,7 +2686,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A54" s="24" t="s">
         <v>33</v>
       </c>
@@ -2518,7 +2707,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>34</v>
       </c>
@@ -2538,8 +2727,11 @@
       <c r="G55" s="11" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I55" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="20" t="s">
         <v>35</v>
       </c>
@@ -2560,7 +2752,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="28" t="s">
         <v>36</v>
       </c>
@@ -2582,8 +2774,14 @@
       <c r="G57" s="31" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="I57" t="s">
+        <v>268</v>
+      </c>
+      <c r="J57" s="37" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
         <v>37</v>
       </c>
@@ -2604,7 +2802,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>65</v>
       </c>
@@ -2626,8 +2824,11 @@
       <c r="G59" s="4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I59" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>38</v>
       </c>
@@ -2648,7 +2849,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="20" t="s">
         <v>39</v>
       </c>
@@ -2669,7 +2870,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>40</v>
       </c>
@@ -2688,7 +2889,7 @@
       </c>
       <c r="G62" s="4"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>41</v>
       </c>
@@ -2708,8 +2909,11 @@
       <c r="G63" s="4" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I63" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
added pytesseract ocr for pdfs/images to the scraper
</commit_message>
<xml_diff>
--- a/data/Cities.xlsx
+++ b/data/Cities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jojo\DataKraken\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194B489C-289D-4367-A533-7635C05B121C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA18FA3D-8875-474B-BAC3-86A334C50264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25560" yWindow="7725" windowWidth="22275" windowHeight="12705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27990" yWindow="5445" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="274">
   <si>
     <t>Name</t>
   </si>
@@ -844,6 +844,9 @@
   </si>
   <si>
     <t>https://www.radiogong.com/aktuelles/coronazahlen-in-der-region</t>
+  </si>
+  <si>
+    <t>https://www.stmgp.bayern.de/coronavirus/</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1215,6 +1218,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1502,7 +1506,7 @@
       <pane xSplit="5" ySplit="30" topLeftCell="G46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1594,7 +1598,7 @@
       <c r="H3" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="38" t="s">
         <v>254</v>
       </c>
     </row>
@@ -1740,6 +1744,9 @@
       <c r="G9" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="I9" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -1766,7 +1773,7 @@
       <c r="H10" s="35" t="s">
         <v>252</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="38" t="s">
         <v>253</v>
       </c>
     </row>
@@ -1897,7 +1904,7 @@
       <c r="G16" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="38" t="s">
         <v>258</v>
       </c>
     </row>
@@ -3011,8 +3018,11 @@
     <hyperlink ref="F57" r:id="rId48" xr:uid="{A0C2A79E-654A-4A6D-AC3B-0294B8668277}"/>
     <hyperlink ref="F59" r:id="rId49" xr:uid="{326AE1F9-6BE8-4CF1-B23E-03EFBB15FF2D}"/>
     <hyperlink ref="F13" r:id="rId50" xr:uid="{72932879-D4F4-4F02-A248-2DB0C2AEA14E}"/>
+    <hyperlink ref="I3" r:id="rId51" xr:uid="{93120B99-FECA-47E9-B05E-94B78793C929}"/>
+    <hyperlink ref="I10" r:id="rId52" xr:uid="{8C97B470-5021-46AA-AD25-695CE1DEE695}"/>
+    <hyperlink ref="I16" r:id="rId53" xr:uid="{DD68CE91-2DE3-46EA-9330-21922542A11E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId51"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
support of pdf and image ocr - tried converting images into black and white so tesseract may have higher accuracy seems to work
</commit_message>
<xml_diff>
--- a/data/Cities.xlsx
+++ b/data/Cities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jojo\DataKraken\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA18FA3D-8875-474B-BAC3-86A334C50264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8246D1E-E93D-4688-85BA-C395C89F0AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="5445" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27750" yWindow="5445" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1506,7 +1506,7 @@
       <pane xSplit="5" ySplit="30" topLeftCell="G46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>